<commit_message>
Excel sobre os jogos
</commit_message>
<xml_diff>
--- a/Imgs_Jogos/Infomações_JOgos.xlsx
+++ b/Imgs_Jogos/Infomações_JOgos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Principe Sayajin\OneDrive\Área de Trabalho\Projeto 2 Modulo\Projeto Game Flix\projeto-gameflix-blue\Imgs_Jogos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7716B3A-6C52-49C2-8836-946B56AC6386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="11115" yWindow="1755" windowWidth="17685" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,100 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Nota Metacritc</t>
+  </si>
+  <si>
+    <t>Classificação</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Ano de Lançamento</t>
+  </si>
+  <si>
+    <t>Produtora</t>
+  </si>
+  <si>
+    <t>Trailler</t>
+  </si>
+  <si>
+    <t>God Of War</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>18 Anos</t>
+  </si>
+  <si>
+    <t>Ação</t>
+  </si>
+  <si>
+    <t>Santa Monica</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CJ_GCPaKywg</t>
+  </si>
+  <si>
+    <t>Persona 5</t>
+  </si>
+  <si>
+    <t>Rpg</t>
+  </si>
+  <si>
+    <t>P-Studio</t>
+  </si>
+  <si>
+    <t>8.7</t>
+  </si>
+  <si>
+    <t>17 Anos</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wPqSkzNNPIg</t>
+  </si>
+  <si>
+    <t>Grand Chase</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>MMO</t>
+  </si>
+  <si>
+    <t>KOG-Studios</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GS2i5xqfoY8</t>
+  </si>
+  <si>
+    <t>Dead Space</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Secfn81KB8k</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +127,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +153,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +441,275 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2008</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2008</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>